<commit_message>
Added regex-based handling for combined WD/INS flags in extract_product_flags_and_filter
</commit_message>
<xml_diff>
--- a/data/quotation_template.xlsx
+++ b/data/quotation_template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29201AB7-656F-7443-ADA3-548C1EB6FE82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D039D3-601F-0245-8179-146225CA360F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="30060" windowHeight="20900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18000" yWindow="880" windowWidth="18000" windowHeight="20920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>ลำดับ</t>
   </si>
@@ -124,6 +124,36 @@
   </si>
   <si>
     <t>Disc.</t>
+  </si>
+  <si>
+    <t>List</t>
+  </si>
+  <si>
+    <t>พ่นสี/อลู</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ins </t>
+  </si>
+  <si>
+    <t>Filter</t>
+  </si>
+  <si>
+    <t>Subtotal</t>
+  </si>
+  <si>
+    <t>Disc</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>ค่าสี</t>
+  </si>
+  <si>
+    <t>ค่าขนส่ง</t>
+  </si>
+  <si>
+    <t>รวมทั้งหมด</t>
   </si>
 </sst>
 </file>
@@ -134,7 +164,7 @@
     <numFmt numFmtId="164" formatCode="[$-107041E]d\ mmm\ yy;@"/>
     <numFmt numFmtId="165" formatCode="#,##0.00;[Red]#,##0.00"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,6 +219,14 @@
       <charset val="222"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="222"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -376,10 +414,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -496,6 +535,39 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -511,36 +583,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -550,18 +598,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="ปกติ 2" xfId="1" xr:uid="{49FEFC8B-4F72-C640-855C-7F72198E5FDE}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -944,8 +991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="Q30" sqref="Q30"/>
+    <sheetView tabSelected="1" topLeftCell="T2" zoomScale="125" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="X14" sqref="X14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -973,31 +1020,31 @@
     <col min="33" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="116.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:29" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="56" t="s">
+    <row r="1" spans="1:31" ht="116.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:31" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57"/>
-      <c r="N2" s="57"/>
-      <c r="O2" s="57"/>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="57"/>
-      <c r="R2" s="58"/>
-    </row>
-    <row r="3" spans="1:29" ht="6.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:29" ht="8.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="68"/>
+      <c r="N2" s="68"/>
+      <c r="O2" s="68"/>
+      <c r="P2" s="68"/>
+      <c r="Q2" s="68"/>
+      <c r="R2" s="69"/>
+    </row>
+    <row r="3" spans="1:31" ht="6.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:31" ht="8.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -1017,7 +1064,7 @@
       <c r="Q4" s="3"/>
       <c r="R4" s="4"/>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A5" s="54" t="s">
         <v>5</v>
       </c>
@@ -1035,13 +1082,13 @@
       <c r="M5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="N5" s="67"/>
-      <c r="O5" s="67"/>
-      <c r="P5" s="67"/>
-      <c r="Q5" s="67"/>
+      <c r="N5" s="66"/>
+      <c r="O5" s="66"/>
+      <c r="P5" s="66"/>
+      <c r="Q5" s="66"/>
       <c r="R5" s="6"/>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A6" s="54" t="s">
         <v>7</v>
       </c>
@@ -1059,13 +1106,13 @@
       <c r="M6" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="N6" s="66"/>
-      <c r="O6" s="66"/>
-      <c r="P6" s="66"/>
-      <c r="Q6" s="66"/>
+      <c r="N6" s="72"/>
+      <c r="O6" s="72"/>
+      <c r="P6" s="72"/>
+      <c r="Q6" s="72"/>
       <c r="R6" s="6"/>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A7" s="54"/>
       <c r="B7" s="55"/>
       <c r="C7" s="55"/>
@@ -1081,13 +1128,13 @@
       <c r="M7" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="N7" s="69"/>
-      <c r="O7" s="69"/>
-      <c r="P7" s="69"/>
-      <c r="Q7" s="69"/>
+      <c r="N7" s="73"/>
+      <c r="O7" s="73"/>
+      <c r="P7" s="73"/>
+      <c r="Q7" s="73"/>
       <c r="R7" s="6"/>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A8" s="54" t="s">
         <v>6</v>
       </c>
@@ -1111,7 +1158,7 @@
       <c r="Q8" s="9"/>
       <c r="R8" s="6"/>
     </row>
-    <row r="9" spans="1:29" ht="8.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:31" ht="8.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
@@ -1131,84 +1178,107 @@
       <c r="Q9" s="9"/>
       <c r="R9" s="10"/>
     </row>
-    <row r="10" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A11" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="61" t="s">
+      <c r="B11" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="62"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="61" t="s">
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="62"/>
-      <c r="I11" s="62"/>
+      <c r="H11" s="56"/>
+      <c r="I11" s="56"/>
       <c r="J11" s="63"/>
       <c r="K11" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="L11" s="61" t="s">
+      <c r="L11" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="M11" s="62"/>
+      <c r="M11" s="56"/>
       <c r="N11" s="63"/>
       <c r="O11" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="P11" s="61" t="s">
+      <c r="P11" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="Q11" s="62"/>
+      <c r="Q11" s="56"/>
       <c r="R11" s="63"/>
-      <c r="V11" s="5"/>
-      <c r="W11" s="5"/>
-      <c r="X11" s="5"/>
-      <c r="Y11" s="5"/>
-      <c r="Z11" s="5"/>
-      <c r="AA11" s="5"/>
-      <c r="AB11" s="5"/>
-      <c r="AC11" s="5"/>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="U11" s="77"/>
+      <c r="V11" s="78" t="s">
+        <v>31</v>
+      </c>
+      <c r="W11" s="79" t="s">
+        <v>32</v>
+      </c>
+      <c r="X11" s="79" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y11" s="79" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z11" s="79" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA11" s="79" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB11" s="79" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC11" s="79" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD11" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE11" s="53" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A12" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="64" t="s">
+      <c r="B12" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="65"/>
-      <c r="D12" s="65"/>
-      <c r="E12" s="65"/>
-      <c r="F12" s="65"/>
-      <c r="G12" s="64" t="s">
+      <c r="C12" s="58"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="65"/>
-      <c r="I12" s="65"/>
-      <c r="J12" s="70"/>
+      <c r="H12" s="58"/>
+      <c r="I12" s="58"/>
+      <c r="J12" s="59"/>
       <c r="K12" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="L12" s="64" t="s">
+      <c r="L12" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="M12" s="65"/>
-      <c r="N12" s="70"/>
+      <c r="M12" s="58"/>
+      <c r="N12" s="59"/>
       <c r="O12" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="P12" s="64" t="s">
+      <c r="P12" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="Q12" s="65"/>
-      <c r="R12" s="70"/>
-    </row>
-    <row r="13" spans="1:29" ht="6.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q12" s="58"/>
+      <c r="R12" s="59"/>
+    </row>
+    <row r="13" spans="1:31" ht="6.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="28"/>
       <c r="B13" s="7"/>
       <c r="G13" s="30"/>
@@ -1222,7 +1292,7 @@
       <c r="Q13" s="21"/>
       <c r="R13" s="6"/>
     </row>
-    <row r="14" spans="1:29" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:31" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="28"/>
       <c r="B14" s="37"/>
       <c r="C14" s="47"/>
@@ -1243,7 +1313,7 @@
       <c r="V14" s="42"/>
       <c r="AC14" s="43"/>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A15" s="28"/>
       <c r="B15" s="7"/>
       <c r="D15" s="5"/>
@@ -1261,7 +1331,7 @@
       <c r="V15" s="42"/>
       <c r="AC15" s="43"/>
     </row>
-    <row r="16" spans="1:29" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:31" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="28"/>
       <c r="B16" s="37"/>
       <c r="C16" s="47"/>
@@ -1512,12 +1582,12 @@
       <c r="D29" s="29"/>
       <c r="G29" s="30"/>
       <c r="J29" s="6"/>
-      <c r="K29" s="75" t="s">
+      <c r="K29" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="L29" s="75"/>
-      <c r="M29" s="75"/>
-      <c r="N29" s="75"/>
+      <c r="L29" s="64"/>
+      <c r="M29" s="64"/>
+      <c r="N29" s="64"/>
       <c r="O29" s="31"/>
       <c r="P29" s="2"/>
       <c r="Q29" s="23"/>
@@ -1528,12 +1598,12 @@
       <c r="B30" s="7"/>
       <c r="G30" s="30"/>
       <c r="J30" s="6"/>
-      <c r="K30" s="76" t="s">
+      <c r="K30" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="L30" s="76"/>
-      <c r="M30" s="76"/>
-      <c r="N30" s="76"/>
+      <c r="L30" s="65"/>
+      <c r="M30" s="65"/>
+      <c r="N30" s="65"/>
       <c r="O30" s="32"/>
       <c r="P30" s="8"/>
       <c r="Q30" s="22"/>
@@ -1543,19 +1613,19 @@
       <c r="Y30" s="5"/>
     </row>
     <row r="31" spans="1:29" ht="22" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="71" t="str">
+      <c r="A31" s="74" t="str">
         <f>BAHTTEXT(Q31)</f>
         <v>ศูนย์บาทถ้วน</v>
       </c>
-      <c r="B31" s="72"/>
-      <c r="C31" s="72"/>
-      <c r="D31" s="72"/>
-      <c r="E31" s="72"/>
-      <c r="F31" s="72"/>
-      <c r="G31" s="72"/>
-      <c r="H31" s="72"/>
-      <c r="I31" s="72"/>
-      <c r="J31" s="73"/>
+      <c r="B31" s="75"/>
+      <c r="C31" s="75"/>
+      <c r="D31" s="75"/>
+      <c r="E31" s="75"/>
+      <c r="F31" s="75"/>
+      <c r="G31" s="75"/>
+      <c r="H31" s="75"/>
+      <c r="I31" s="75"/>
+      <c r="J31" s="76"/>
       <c r="K31" s="55" t="s">
         <v>22</v>
       </c>
@@ -1572,81 +1642,70 @@
       <c r="A33" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D33" s="67"/>
-      <c r="E33" s="67"/>
-      <c r="F33" s="67"/>
-      <c r="G33" s="67"/>
-      <c r="H33" s="67"/>
-      <c r="I33" s="67"/>
-      <c r="J33" s="67"/>
-      <c r="K33" s="67"/>
-      <c r="M33" s="60"/>
-      <c r="N33" s="60"/>
-      <c r="O33" s="60"/>
-      <c r="P33" s="60"/>
-      <c r="Q33" s="60"/>
+      <c r="D33" s="66"/>
+      <c r="E33" s="66"/>
+      <c r="F33" s="66"/>
+      <c r="G33" s="66"/>
+      <c r="H33" s="66"/>
+      <c r="I33" s="66"/>
+      <c r="J33" s="66"/>
+      <c r="K33" s="66"/>
+      <c r="M33" s="71"/>
+      <c r="N33" s="71"/>
+      <c r="O33" s="71"/>
+      <c r="P33" s="71"/>
+      <c r="Q33" s="71"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F34" s="68"/>
-      <c r="G34" s="68"/>
-      <c r="H34" s="68"/>
-      <c r="I34" s="68"/>
-      <c r="J34" s="68"/>
-      <c r="K34" s="68"/>
-      <c r="M34" s="59" t="s">
+      <c r="F34" s="61"/>
+      <c r="G34" s="61"/>
+      <c r="H34" s="61"/>
+      <c r="I34" s="61"/>
+      <c r="J34" s="61"/>
+      <c r="K34" s="61"/>
+      <c r="M34" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="N34" s="59"/>
-      <c r="O34" s="59"/>
-      <c r="P34" s="59"/>
-      <c r="Q34" s="59"/>
+      <c r="N34" s="70"/>
+      <c r="O34" s="70"/>
+      <c r="P34" s="70"/>
+      <c r="Q34" s="70"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F35" s="68"/>
-      <c r="G35" s="68"/>
-      <c r="H35" s="68"/>
-      <c r="I35" s="68"/>
-      <c r="J35" s="68"/>
-      <c r="K35" s="68"/>
+      <c r="F35" s="61"/>
+      <c r="G35" s="61"/>
+      <c r="H35" s="61"/>
+      <c r="I35" s="61"/>
+      <c r="J35" s="61"/>
+      <c r="K35" s="61"/>
       <c r="O35" s="1"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="F36" s="74"/>
-      <c r="G36" s="68"/>
-      <c r="H36" s="68"/>
-      <c r="I36" s="68"/>
-      <c r="J36" s="68"/>
-      <c r="K36" s="68"/>
-      <c r="M36" s="62" t="s">
+      <c r="F36" s="60"/>
+      <c r="G36" s="61"/>
+      <c r="H36" s="61"/>
+      <c r="I36" s="61"/>
+      <c r="J36" s="61"/>
+      <c r="K36" s="61"/>
+      <c r="M36" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="N36" s="62"/>
-      <c r="O36" s="62"/>
-      <c r="P36" s="62"/>
-      <c r="Q36" s="62"/>
+      <c r="N36" s="56"/>
+      <c r="O36" s="56"/>
+      <c r="P36" s="56"/>
+      <c r="Q36" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="M36:Q36"/>
-    <mergeCell ref="L12:N12"/>
-    <mergeCell ref="F36:K36"/>
-    <mergeCell ref="P11:R11"/>
-    <mergeCell ref="P12:R12"/>
-    <mergeCell ref="K29:N29"/>
-    <mergeCell ref="K30:N30"/>
-    <mergeCell ref="K31:N31"/>
-    <mergeCell ref="F35:K35"/>
-    <mergeCell ref="D33:K33"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A2:R2"/>
     <mergeCell ref="M34:Q34"/>
@@ -1663,6 +1722,17 @@
     <mergeCell ref="G12:J12"/>
     <mergeCell ref="A31:J31"/>
     <mergeCell ref="L11:N11"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="M36:Q36"/>
+    <mergeCell ref="L12:N12"/>
+    <mergeCell ref="F36:K36"/>
+    <mergeCell ref="P11:R11"/>
+    <mergeCell ref="P12:R12"/>
+    <mergeCell ref="K29:N29"/>
+    <mergeCell ref="K30:N30"/>
+    <mergeCell ref="K31:N31"/>
+    <mergeCell ref="F35:K35"/>
+    <mergeCell ref="D33:K33"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.51181102362204722" right="0.31496062992125984" top="0.19685039370078741" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>